<commit_message>
updated basetest, Email Integration done
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6950" tabRatio="864" firstSheet="1" activeTab="4"/>
+    <workbookView windowWidth="19200" windowHeight="6950" tabRatio="864" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin_myschool" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="181">
   <si>
     <t>Username</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>123456</t>
+  </si>
+  <si>
+    <t>three.9393688889</t>
+  </si>
+  <si>
+    <t>Taut@2023</t>
   </si>
   <si>
     <t>codewave</t>
@@ -1581,8 +1587,8 @@
   <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -1608,8 +1614,12 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="9"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="9"/>
@@ -1617,7 +1627,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="mithun@codewave.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="mithun@codewave.com" tooltip="mailto:mithun@codewave.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -1649,18 +1659,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1705,55 +1715,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="Q1" s="11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -1764,52 +1774,52 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="P2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="Q2" s="13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="R2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -1820,52 +1830,52 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="N3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="O3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="P3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="Q3" s="13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="R3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1888,7 +1898,7 @@
   <sheetPr/>
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1919,61 +1929,61 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -1984,58 +1994,58 @@
         <v>3</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="J2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="O2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="P2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="S2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="T2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -2046,58 +2056,58 @@
         <v>3</v>
       </c>
       <c r="C3" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" t="s">
+        <v>78</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="L3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M3" t="s">
+        <v>81</v>
+      </c>
+      <c r="N3" t="s">
+        <v>82</v>
+      </c>
+      <c r="O3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>85</v>
+      </c>
+      <c r="R3" t="s">
+        <v>86</v>
+      </c>
+      <c r="S3" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="T3" t="s">
         <v>88</v>
-      </c>
-      <c r="E3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="H3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" t="s">
-        <v>76</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="L3" t="s">
-        <v>78</v>
-      </c>
-      <c r="M3" t="s">
-        <v>79</v>
-      </c>
-      <c r="N3" t="s">
-        <v>80</v>
-      </c>
-      <c r="O3" t="s">
-        <v>81</v>
-      </c>
-      <c r="P3" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>83</v>
-      </c>
-      <c r="R3" t="s">
-        <v>84</v>
-      </c>
-      <c r="S3" t="s">
-        <v>85</v>
-      </c>
-      <c r="T3" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2152,61 +2162,61 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -2217,58 +2227,58 @@
         <v>3</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" t="s">
-        <v>90</v>
-      </c>
       <c r="G2" s="15" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="J2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="O2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="P2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="S2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="T2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -2279,58 +2289,58 @@
         <v>3</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="J3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="O3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="P3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="S3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="T3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2363,61 +2373,61 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -2428,58 +2438,58 @@
         <v>3</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="J2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="O2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="P2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="S2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="T2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2499,7 +2509,7 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -2517,7 +2527,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2525,7 +2535,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -2533,39 +2543,39 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -2573,74 +2583,74 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -2667,58 +2677,58 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -2726,55 +2736,55 @@
         <v>1005</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C19" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F19" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G19" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H19" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="I19">
         <v>600001</v>
       </c>
       <c r="J19" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="K19" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L19" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="M19" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="N19" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="O19" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="P19" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="Q19" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="R19" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -2782,55 +2792,55 @@
         <v>1006</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C20" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D20" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G20" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I20">
         <v>560010</v>
       </c>
       <c r="J20" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K20" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L20" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="M20" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="N20" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="O20" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="P20" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="Q20" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="R20" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -2838,55 +2848,55 @@
         <v>1007</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C21" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G21" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H21" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="I21">
         <v>572101</v>
       </c>
       <c r="J21" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="K21" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L21" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="M21" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="N21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="O21" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="P21" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="Q21" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="R21" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -2894,55 +2904,55 @@
         <v>1008</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C22" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="F22" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G22" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H22" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I22">
         <v>560010</v>
       </c>
       <c r="J22" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="K22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L22" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="M22" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="N22" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="O22" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="P22" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="Q22" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="R22" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -2950,66 +2960,66 @@
         <v>1009</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C23" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F23" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H23" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="I23">
         <v>600001</v>
       </c>
       <c r="J23" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="K23" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L23" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="M23" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="N23" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="O23" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="P23" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="Q23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="R23" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="14:16">
       <c r="N24" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="P24" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="2:21">
@@ -3042,55 +3052,55 @@
         <v>0</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M27" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N27" s="8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="Q27" s="11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -3101,52 +3111,52 @@
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F28" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="I28" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="J28" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="L28" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M28" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="N28" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="O28" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="P28" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="Q28" s="13" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="R28" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -3157,52 +3167,52 @@
         <v>5</v>
       </c>
       <c r="C29" t="s">
+        <v>171</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="F29" t="s">
+        <v>174</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="I29" t="s">
+        <v>177</v>
+      </c>
+      <c r="J29" t="s">
+        <v>35</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="L29" t="s">
+        <v>37</v>
+      </c>
+      <c r="M29" t="s">
+        <v>179</v>
+      </c>
+      <c r="N29" t="s">
+        <v>180</v>
+      </c>
+      <c r="O29" t="s">
+        <v>168</v>
+      </c>
+      <c r="P29" t="s">
         <v>169</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="Q29" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="E29" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F29" t="s">
-        <v>172</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="H29" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="I29" t="s">
-        <v>175</v>
-      </c>
-      <c r="J29" t="s">
-        <v>33</v>
-      </c>
-      <c r="K29" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="L29" t="s">
-        <v>35</v>
-      </c>
-      <c r="M29" t="s">
-        <v>177</v>
-      </c>
-      <c r="N29" t="s">
-        <v>178</v>
-      </c>
-      <c r="O29" t="s">
-        <v>166</v>
-      </c>
-      <c r="P29" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q29" s="13" t="s">
-        <v>168</v>
-      </c>
       <c r="R29" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="2:9">

</xml_diff>